<commit_message>
fix validate profile, route, and regional
</commit_message>
<xml_diff>
--- a/public/storage/document/import_alumni.xlsx
+++ b/public/storage/document/import_alumni.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Eduraya\Sistem Alumni UNS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3353C39C-A197-440E-83DA-85212C8662C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6255D481-8D47-43CE-ABE3-B854B4DE8DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A75038FC-36C5-4306-B2D4-67C670F4F1AC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>Nala</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>jurusan_id</t>
+  </si>
+  <si>
+    <t>negara</t>
+  </si>
+  <si>
+    <t>provinsi</t>
+  </si>
+  <si>
+    <t>kabupaten</t>
+  </si>
+  <si>
+    <t>kecamatan</t>
   </si>
 </sst>
 </file>
@@ -536,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9E6D99-0E45-466E-9417-FD156A5585C8}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,17 +563,19 @@
     <col min="5" max="5" width="17.21875" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5546875" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.21875" customWidth="1"/>
-    <col min="14" max="14" width="16.88671875" customWidth="1"/>
-    <col min="15" max="15" width="16.5546875" customWidth="1"/>
-    <col min="16" max="16" width="20.109375" customWidth="1"/>
-    <col min="17" max="18" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" customWidth="1"/>
+    <col min="9" max="11" width="12" customWidth="1"/>
+    <col min="13" max="13" width="18.5546875" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" customWidth="1"/>
+    <col min="17" max="17" width="15.21875" customWidth="1"/>
+    <col min="18" max="18" width="16.88671875" customWidth="1"/>
+    <col min="19" max="19" width="16.5546875" customWidth="1"/>
+    <col min="20" max="20" width="20.109375" customWidth="1"/>
+    <col min="21" max="22" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -584,40 +598,52 @@
         <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,39 +665,43 @@
       <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1">
+      <c r="N2" s="1">
         <v>1</v>
       </c>
-      <c r="K2" s="1">
+      <c r="O2" s="1">
         <v>3</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="1"/>
+      <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -693,33 +723,37 @@
       <c r="G3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="1">
+      <c r="N3" s="1">
         <v>1</v>
       </c>
-      <c r="K3" s="1">
+      <c r="O3" s="1">
         <v>3</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
+      <c r="U3" s="1"/>
+      <c r="V3" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -743,25 +777,29 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1">
         <v>1</v>
       </c>
-      <c r="K4" s="1">
+      <c r="O4" s="1">
         <v>3</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>